<commit_message>
Removed params and returns types
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="C113" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="C111" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="C114" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="C112" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="C115" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="C115" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="C112" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="C114" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="C111" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="C113" sheetId="5" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -465,22 +465,22 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Profesor:Yudivian
-Asignatura:Logica
-Aula:3</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
           <t>Profesor:DanielL
 Asignatura:LogicaCp
 Aula:4</t>
         </is>
       </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Profesor:DalianisAL
+Asignatura:AlgebraCP
+Aula:3</t>
+        </is>
+      </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Profesor:Piad
-Asignatura:Programacion
+          <t>Profesor:PacoP
+Asignatura:ProgramacionCp
 Aula:2</t>
         </is>
       </c>
@@ -499,60 +499,60 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Profesor:CristinaA
-Asignatura:AnalisisCp
-Aula:5</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Profesor:CayetanaAL
-Asignatura:AlgebraCP
-Aula:4</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
           <t>Profesor:CarlaP
 Asignatura:ProgramacionCp
-Aula:2</t>
+Aula:1</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Profesor:Piad
+Asignatura:Programacion
+Aula:1</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Profesor:ErnestoA
+Asignatura:AnalisisCp
+Aula:4</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
-        <is>
-          <t>Profesor:HectorP
-Asignatura:ProgramacionCp
-Aula:5</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
         <is>
           <t>Profesor:Idania
 Asignatura:Analisis
 Aula:3</t>
         </is>
       </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Profesor:Celia
+Asignatura:Algebra
+Aula:3</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Profesor:ErnestoA
-Asignatura:AnalisisCp
-Aula:4</t>
-        </is>
-      </c>
+      <c r="B4" t="inlineStr"/>
       <c r="C4" t="inlineStr"/>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Profesor:Celia
-Asignatura:Algebra
-Aula:2</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr"/>
+          <t>Profesor:Yudivian
+Asignatura:Logica
+Aula:2</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Profesor:CristinaA
+Asignatura:AnalisisCp
+Aula:1</t>
+        </is>
+      </c>
       <c r="F4" t="inlineStr"/>
     </row>
   </sheetData>
@@ -602,71 +602,71 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
+          <t>Profesor:Idania
+Asignatura:Analisis
+Aula:2</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Profesor:CayetanaAL
+Asignatura:AlgebraCP
+Aula:5</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Profesor:Piad
+Asignatura:Programacion
+Aula:4</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Profesor:CristinaA
+Asignatura:AnalisisCp
+Aula:1</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Profesor:HectorP
+Asignatura:ProgramacionCp
+Aula:3</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
           <t>Profesor:DanielL
 Asignatura:LogicaCp
 Aula:5</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Profesor:CarlaP
+Asignatura:ProgramacionCp
+Aula:2</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
         <is>
           <t>Profesor:Celia
 Asignatura:Algebra
-Aula:3</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>Profesor:CarlaP
-Asignatura:ProgramacionCp
 Aula:5</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>Profesor:CarlaP
-Asignatura:ProgramacionCp
-Aula:5</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr"/>
-    </row>
-    <row r="3">
-      <c r="A3" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Profesor:DalianisAL
-Asignatura:AlgebraCP
-Aula:3</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Profesor:CristinaA
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Profesor:MercedesA
 Asignatura:AnalisisCp
-Aula:3</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>Profesor:PepeAl
-Asignatura:AlgebraCP
-Aula:4</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>Profesor:Yudivian
-Asignatura:Logica
-Aula:2</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>Profesor:Piad
-Asignatura:Programacion
-Aula:4</t>
+Aula:2</t>
         </is>
       </c>
     </row>
@@ -677,20 +677,20 @@
       <c r="B4" t="inlineStr"/>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Profesor:ErnestoA
-Asignatura:AnalisisCp
-Aula:3</t>
+          <t>Profesor:Yudivian
+Asignatura:Logica
+Aula:2</t>
         </is>
       </c>
       <c r="D4" t="inlineStr"/>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>Profesor:Idania
-Asignatura:Analisis
-Aula:2</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr"/>
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Profesor:PepeAl
+Asignatura:AlgebraCP
+Aula:1</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -739,30 +739,30 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
+          <t>Profesor:Celia
+Asignatura:Algebra
+Aula:1</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
           <t>Profesor:Piad
 Asignatura:Programacion
 Aula:4</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Profesor:MercedesA
-Asignatura:AnalisisCp
-Aula:1</t>
-        </is>
-      </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Profesor:DanielL
-Asignatura:LogicaCp
-Aula:3</t>
+          <t>Profesor:PepeAl
+Asignatura:AlgebraCP
+Aula:1</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Profesor:CayetanaAL
-Asignatura:AlgebraCP
-Aula:3</t>
+          <t>Profesor:Yudivian
+Asignatura:Logica
+Aula:2</t>
         </is>
       </c>
       <c r="F2" t="inlineStr"/>
@@ -773,37 +773,37 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Profesor:Yudivian
-Asignatura:Logica
+          <t>Profesor:CayetanaAL
+Asignatura:AlgebraCP
 Aula:2</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Profesor:CarlaP
+          <t>Profesor:Idania
+Asignatura:Analisis
+Aula:2</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Profesor:PacoP
 Asignatura:ProgramacionCp
 Aula:5</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>Profesor:DalianisAL
-Asignatura:AlgebraCP
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Profesor:OmarL
+Asignatura:LogicaCp
 Aula:4</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>Profesor:Celia
-Asignatura:Algebra
-Aula:4</t>
-        </is>
-      </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Profesor:Idania
-Asignatura:Analisis
-Aula:3</t>
+          <t>Profesor:MercedesA
+Asignatura:AnalisisCp
+Aula:2</t>
         </is>
       </c>
     </row>
@@ -811,20 +811,20 @@
       <c r="A4" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="B4" t="inlineStr"/>
-      <c r="C4" t="inlineStr"/>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>Profesor:MercedesA
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Profesor:CristinaA
 Asignatura:AnalisisCp
 Aula:4</t>
         </is>
       </c>
+      <c r="C4" t="inlineStr"/>
+      <c r="D4" t="inlineStr"/>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Profesor:PacoP
+          <t>Profesor:HectorP
 Asignatura:ProgramacionCp
-Aula:1</t>
+Aula:4</t>
         </is>
       </c>
       <c r="F4" t="inlineStr"/>
@@ -876,30 +876,30 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Profesor:Idania
-Asignatura:Analisis
-Aula:2</t>
+          <t>Profesor:Celia
+Asignatura:Algebra
+Aula:1</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Profesor:OmarL
+          <t>Profesor:DanielL
 Asignatura:LogicaCp
-Aula:2</t>
+Aula:1</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
-        <is>
-          <t>Profesor:Yudivian
-Asignatura:Logica
-Aula:1</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
         <is>
           <t>Profesor:ErnestoA
 Asignatura:AnalisisCp
-Aula:1</t>
+Aula:5</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Profesor:CayetanaAL
+Asignatura:AlgebraCP
+Aula:3</t>
         </is>
       </c>
       <c r="F2" t="inlineStr"/>
@@ -910,36 +910,36 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Profesor:CayetanaAL
-Asignatura:AlgebraCP
+          <t>Profesor:CarlaP
+Asignatura:ProgramacionCp
+Aula:1</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Profesor:Yudivian
+Asignatura:Logica
 Aula:3</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Profesor:DalianisAL
-Asignatura:AlgebraCP
-Aula:1</t>
-        </is>
-      </c>
       <c r="D3" t="inlineStr">
+        <is>
+          <t>Profesor:MercedesA
+Asignatura:AnalisisCp
+Aula:3</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
         <is>
           <t>Profesor:HectorP
 Asignatura:ProgramacionCp
-Aula:3</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>Profesor:Celia
-Asignatura:Algebra
-Aula:4</t>
+Aula:1</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Profesor:MercedesA
-Asignatura:AnalisisCp
+          <t>Profesor:PepeAl
+Asignatura:AlgebraCP
 Aula:1</t>
         </is>
       </c>
@@ -949,22 +949,22 @@
         <v>3</v>
       </c>
       <c r="B4" t="inlineStr"/>
-      <c r="C4" t="inlineStr"/>
-      <c r="D4" t="inlineStr">
+      <c r="C4" t="inlineStr">
         <is>
           <t>Profesor:Piad
 Asignatura:Programacion
 Aula:5</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr"/>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>Profesor:CarlaP
-Asignatura:ProgramacionCp
+      <c r="D4" t="inlineStr"/>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Profesor:Idania
+Asignatura:Analisis
 Aula:5</t>
         </is>
       </c>
+      <c r="F4" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1013,32 +1013,32 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Profesor:Yudivian
-Asignatura:Logica
-Aula:3</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
           <t>Profesor:CarmenL
 Asignatura:LogicaCp
 Aula:4</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>Profesor:CarlaP
-Asignatura:ProgramacionCp
-Aula:5</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
+      <c r="C2" t="inlineStr">
         <is>
           <t>Profesor:PepeAl
 Asignatura:AlgebraCP
 Aula:3</t>
         </is>
       </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Profesor:ErnestoA
+Asignatura:AnalisisCp
+Aula:5</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Profesor:Yudivian
+Asignatura:Logica
+Aula:2</t>
+        </is>
+      </c>
       <c r="F2" t="inlineStr"/>
     </row>
     <row r="3">
@@ -1047,36 +1047,36 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Profesor:CristinaA
+          <t>Profesor:MercedesA
 Asignatura:AnalisisCp
 Aula:5</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
+          <t>Profesor:CayetanaAL
+Asignatura:AlgebraCP
+Aula:4</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Profesor:CarlaP
+Asignatura:ProgramacionCp
+Aula:2</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Profesor:CarlaP
+Asignatura:ProgramacionCp
+Aula:1</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
           <t>Profesor:Celia
 Asignatura:Algebra
-Aula:2</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>Profesor:PacoP
-Asignatura:ProgramacionCp
-Aula:2</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>Profesor:PepeAl
-Asignatura:AlgebraCP
-Aula:3</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>Profesor:Idania
-Asignatura:Analisis
 Aula:3</t>
         </is>
       </c>
@@ -1087,19 +1087,19 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
+          <t>Profesor:Idania
+Asignatura:Analisis
+Aula:2</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
           <t>Profesor:Piad
 Asignatura:Programacion
 Aula:5</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr"/>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>Profesor:MercedesA
-Asignatura:AnalisisCp
-Aula:4</t>
-        </is>
-      </c>
+      <c r="D4" t="inlineStr"/>
       <c r="E4" t="inlineStr"/>
       <c r="F4" t="inlineStr"/>
     </row>

</xml_diff>